<commit_message>
# fix bug not display ac status 's pt.
</commit_message>
<xml_diff>
--- a/vst/ptaudit/cim.xlsx
+++ b/vst/ptaudit/cim.xlsx
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="181">
   <si>
     <t>gplblmt.p</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -710,6 +710,61 @@
   </si>
   <si>
     <t>CH</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>var_pmc_noconf</t>
+  </si>
+  <si>
+    <t>var_pur_noconf</t>
+  </si>
+  <si>
+    <t>var_eng_noconf</t>
+  </si>
+  <si>
+    <t>var_doc_noconf</t>
+  </si>
+  <si>
+    <t>var_fin_noconf</t>
+  </si>
+  <si>
+    <t>PMC_NO_CONFIRM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PUR_NO_CONFIRM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ENG_NO_CONFIRM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DOC_NO_CONFIRM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FIN_NO_CONFIRM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PMC未确认</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>采购未确认</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>工艺未确认</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R&amp;D未确认</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>财务未确认</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1110,17 +1165,17 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.25" customWidth="1"/>
     <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
@@ -1304,6 +1359,61 @@
       </c>
       <c r="C11" t="s">
         <v>164</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" t="s">
+        <v>171</v>
+      </c>
+      <c r="C12" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" t="s">
+        <v>172</v>
+      </c>
+      <c r="C13" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" t="s">
+        <v>173</v>
+      </c>
+      <c r="C14" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" t="s">
+        <v>174</v>
+      </c>
+      <c r="C15" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" t="s">
+        <v>175</v>
+      </c>
+      <c r="C16" t="s">
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -1331,11 +1441,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C70"/>
+  <dimension ref="A1:C75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B69" sqref="B69"/>
+      <pane ySplit="4" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B71" sqref="B71:B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1983,10 +2093,65 @@
         <v>161</v>
       </c>
     </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A71" t="s">
+        <v>166</v>
+      </c>
+      <c r="B71" t="s">
+        <v>147</v>
+      </c>
+      <c r="C71" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A72" t="s">
+        <v>167</v>
+      </c>
+      <c r="B72" t="s">
+        <v>147</v>
+      </c>
+      <c r="C72" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A73" t="s">
+        <v>168</v>
+      </c>
+      <c r="B73" t="s">
+        <v>147</v>
+      </c>
+      <c r="C73" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A74" t="s">
+        <v>169</v>
+      </c>
+      <c r="B74" t="s">
+        <v>147</v>
+      </c>
+      <c r="C74" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A75" t="s">
+        <v>170</v>
+      </c>
+      <c r="B75" t="s">
+        <v>147</v>
+      </c>
+      <c r="C75" t="s">
+        <v>175</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="textLength" imeMode="off" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="数据长度错误" error="数据长度必须在6-35个字符之间" sqref="C39:C43 C45:C49 C15:C19 C57:C61 C68">
+    <dataValidation type="textLength" imeMode="off" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="数据长度错误" error="数据长度必须在6-35个字符之间" sqref="C39:C43 C45:C49 C15:C19 C57:C61 C68 C71:C75">
       <formula1>6</formula1>
       <formula2>35</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
# update vst program.
</commit_message>
<xml_diff>
--- a/vst/ptaudit/cim.xlsx
+++ b/vst/ptaudit/cim.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="12780" windowHeight="6045" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="12780" windowHeight="6045" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="~gplblmt.p" sheetId="2" r:id="rId1"/>
     <sheet name="gplbldmt.p" sheetId="3" r:id="rId2"/>
     <sheet name="mgflpwmt.p" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -1443,9 +1443,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="4" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B71" sqref="B71:B75"/>
+      <selection pane="bottomLeft" activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2164,8 +2164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>